<commit_message>
Baseline solving A* method.
</commit_message>
<xml_diff>
--- a/Data/Maps/Basic.xlsx
+++ b/Data/Maps/Basic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\SokobanDotNet\Data\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7119EBC4-DF5C-41E7-B949-D1B167C2D46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BE5EBB-EB65-4B51-82EA-DCB38524F803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{6D6D78AC-9F15-486B-9C60-E5063833B960}"/>
+    <workbookView xWindow="38470" yWindow="19820" windowWidth="21460" windowHeight="12440" xr2:uid="{6D6D78AC-9F15-486B-9C60-E5063833B960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>